<commit_message>
setDataIntoExcel method created in Excel Utiility
</commit_message>
<xml_diff>
--- a/NinzaHRMProject/TestData/testScriptData.xlsx
+++ b/NinzaHRMProject/TestData/testScriptData.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Harshali\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D562A37-395B-41DB-90B1-F09B76456695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{238B3D11-FED1-4DFB-9BE2-0114D5599161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="org" sheetId="1" r:id="rId1"/>
@@ -18,9 +13,10 @@
     <sheet name="project" sheetId="3" r:id="rId3"/>
     <sheet name="contact" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:N16"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>TC_ID</t>
   </si>
@@ -154,12 +150,19 @@
   </si>
   <si>
     <t>9369496496</t>
+  </si>
+  <si>
+    <t>SetValue-Working</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,9 +490,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.453125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -635,16 +638,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EC755E-6E42-44EB-B677-CBA716B3C2EA}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -671,12 +674,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -694,9 +704,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.90625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -738,15 +748,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA33078-1E05-4DC7-B960-ABD554B9DF19}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.453125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>